<commit_message>
Allow to display data in a date table in Excel exports.
</commit_message>
<xml_diff>
--- a/emr/exports/templates/export-template-detail.xlsx
+++ b/emr/exports/templates/export-template-detail.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="174">
   <si>
     <t>Date</t>
   </si>
@@ -573,6 +573,9 @@
   </si>
   <si>
     <t>datetable</t>
+  </si>
+  <si>
+    <t>Type Reference</t>
   </si>
 </sst>
 </file>
@@ -1541,8 +1544,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="37">
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2154,7 +2169,55 @@
     <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="14" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2163,102 +2226,54 @@
     <xf numFmtId="1" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2418,39 +2433,39 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2467,7 +2482,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2484,6 +2499,8 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2500,6 +2517,8 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3960,19 +3979,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="9.1640625" style="153" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="153"/>
+    <col min="3" max="9" width="10.83203125" style="153"/>
+    <col min="10" max="10" width="12.5" style="153" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="153"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="152" customFormat="1" ht="11">
+    <row r="1" spans="1:10" s="152" customFormat="1" ht="11">
       <c r="A1" s="152" t="s">
         <v>120</v>
       </c>
@@ -3997,8 +4018,11 @@
       <c r="I1" s="152" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="11">
+      <c r="J1" s="152" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="11">
       <c r="A2" s="153">
         <v>1</v>
       </c>
@@ -4020,11 +4044,8 @@
       <c r="H2" s="153">
         <v>14</v>
       </c>
-      <c r="I2" s="153" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="11">
+    </row>
+    <row r="3" spans="1:10" ht="11">
       <c r="A3" s="153">
         <v>2</v>
       </c>
@@ -4049,8 +4070,11 @@
       <c r="I3" s="153" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="11">
+      <c r="J3" s="153" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="11">
       <c r="D4" s="153">
         <v>1</v>
       </c>
@@ -4069,8 +4093,11 @@
       <c r="I4" s="153" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="11">
+      <c r="J4" s="153" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="11">
       <c r="D5" s="153">
         <v>1</v>
       </c>
@@ -4089,8 +4116,11 @@
       <c r="I5" s="153" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="11">
+      <c r="J5" s="153" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="11">
       <c r="D6" s="153">
         <v>1</v>
       </c>
@@ -4109,8 +4139,11 @@
       <c r="I6" s="153" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="11">
+      <c r="J6" s="153" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="11">
       <c r="D7" s="153">
         <v>1</v>
       </c>
@@ -4129,8 +4162,11 @@
       <c r="I7" s="153" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="11">
+      <c r="J7" s="153" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="11">
       <c r="D8" s="153">
         <v>1</v>
       </c>
@@ -4150,7 +4186,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14" customHeight="1">
+    <row r="9" spans="1:10" ht="14" customHeight="1">
       <c r="D9" s="153">
         <v>1</v>
       </c>
@@ -4170,7 +4206,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" customHeight="1">
+    <row r="10" spans="1:10" ht="14" customHeight="1">
       <c r="D10" s="153">
         <v>1</v>
       </c>
@@ -4190,7 +4226,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14" customHeight="1">
+    <row r="11" spans="1:10" ht="14" customHeight="1">
       <c r="D11" s="153">
         <v>1</v>
       </c>
@@ -4207,7 +4243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" customHeight="1">
+    <row r="12" spans="1:10" ht="14" customHeight="1">
       <c r="D12" s="153">
         <v>1</v>
       </c>
@@ -4224,7 +4260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14" customHeight="1">
+    <row r="13" spans="1:10" ht="14" customHeight="1">
       <c r="D13" s="153">
         <v>1</v>
       </c>
@@ -4244,7 +4280,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" customHeight="1">
+    <row r="14" spans="1:10" ht="14" customHeight="1">
       <c r="D14" s="153">
         <v>1</v>
       </c>
@@ -4261,7 +4297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14" customHeight="1">
+    <row r="15" spans="1:10" ht="14" customHeight="1">
       <c r="D15" s="153">
         <v>1</v>
       </c>
@@ -4281,7 +4317,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14" customHeight="1">
+    <row r="16" spans="1:10" ht="14" customHeight="1">
       <c r="D16" s="153">
         <v>2</v>
       </c>
@@ -5578,22 +5614,22 @@
         <v>77</v>
       </c>
       <c r="W30" s="232"/>
-      <c r="X30" s="201" t="s">
+      <c r="X30" s="203" t="s">
         <v>78</v>
       </c>
-      <c r="Y30" s="201"/>
-      <c r="Z30" s="201" t="s">
+      <c r="Y30" s="203"/>
+      <c r="Z30" s="203" t="s">
         <v>79</v>
       </c>
-      <c r="AA30" s="201"/>
-      <c r="AB30" s="201" t="s">
+      <c r="AA30" s="203"/>
+      <c r="AB30" s="203" t="s">
         <v>80</v>
       </c>
-      <c r="AC30" s="201"/>
-      <c r="AD30" s="201" t="s">
+      <c r="AC30" s="203"/>
+      <c r="AD30" s="203" t="s">
         <v>82</v>
       </c>
-      <c r="AE30" s="202"/>
+      <c r="AE30" s="204"/>
     </row>
     <row r="31" spans="1:57" ht="15" customHeight="1" thickTop="1">
       <c r="A31" s="241"/>
@@ -5907,24 +5943,24 @@
       <c r="M39" s="245"/>
       <c r="N39" s="246"/>
       <c r="O39" s="110"/>
-      <c r="P39" s="198" t="s">
+      <c r="P39" s="180" t="s">
         <v>57</v>
       </c>
-      <c r="Q39" s="199"/>
-      <c r="R39" s="199"/>
-      <c r="S39" s="199"/>
-      <c r="T39" s="199"/>
-      <c r="U39" s="199"/>
-      <c r="V39" s="200"/>
-      <c r="W39" s="200"/>
-      <c r="X39" s="174"/>
-      <c r="Y39" s="174"/>
-      <c r="Z39" s="174"/>
-      <c r="AA39" s="174"/>
-      <c r="AB39" s="174"/>
-      <c r="AC39" s="174"/>
-      <c r="AD39" s="174"/>
-      <c r="AE39" s="175"/>
+      <c r="Q39" s="181"/>
+      <c r="R39" s="181"/>
+      <c r="S39" s="181"/>
+      <c r="T39" s="181"/>
+      <c r="U39" s="181"/>
+      <c r="V39" s="182"/>
+      <c r="W39" s="182"/>
+      <c r="X39" s="183"/>
+      <c r="Y39" s="183"/>
+      <c r="Z39" s="183"/>
+      <c r="AA39" s="183"/>
+      <c r="AB39" s="183"/>
+      <c r="AC39" s="183"/>
+      <c r="AD39" s="183"/>
+      <c r="AE39" s="205"/>
     </row>
     <row r="40" spans="1:31" ht="9.75" customHeight="1" thickBot="1">
       <c r="A40" s="77"/>
@@ -6004,40 +6040,40 @@
       </c>
       <c r="D42" s="75"/>
       <c r="E42" s="110"/>
-      <c r="F42" s="172" t="s">
+      <c r="F42" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="G42" s="173"/>
-      <c r="H42" s="173"/>
-      <c r="I42" s="172" t="s">
+      <c r="G42" s="189"/>
+      <c r="H42" s="189"/>
+      <c r="I42" s="188" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="173"/>
-      <c r="K42" s="173"/>
-      <c r="L42" s="173"/>
-      <c r="M42" s="173"/>
-      <c r="N42" s="173"/>
-      <c r="O42" s="173"/>
-      <c r="P42" s="173"/>
-      <c r="Q42" s="172" t="s">
+      <c r="J42" s="189"/>
+      <c r="K42" s="189"/>
+      <c r="L42" s="189"/>
+      <c r="M42" s="189"/>
+      <c r="N42" s="189"/>
+      <c r="O42" s="189"/>
+      <c r="P42" s="189"/>
+      <c r="Q42" s="188" t="s">
         <v>43</v>
       </c>
-      <c r="R42" s="173"/>
+      <c r="R42" s="189"/>
       <c r="S42" s="215"/>
-      <c r="T42" s="173" t="s">
+      <c r="T42" s="189" t="s">
         <v>44</v>
       </c>
-      <c r="U42" s="173"/>
-      <c r="V42" s="173"/>
-      <c r="W42" s="173"/>
-      <c r="X42" s="173"/>
-      <c r="Y42" s="173"/>
-      <c r="Z42" s="173"/>
-      <c r="AA42" s="173"/>
-      <c r="AB42" s="173"/>
-      <c r="AC42" s="173"/>
-      <c r="AD42" s="173"/>
-      <c r="AE42" s="176"/>
+      <c r="U42" s="189"/>
+      <c r="V42" s="189"/>
+      <c r="W42" s="189"/>
+      <c r="X42" s="189"/>
+      <c r="Y42" s="189"/>
+      <c r="Z42" s="189"/>
+      <c r="AA42" s="189"/>
+      <c r="AB42" s="189"/>
+      <c r="AC42" s="189"/>
+      <c r="AD42" s="189"/>
+      <c r="AE42" s="190"/>
     </row>
     <row r="43" spans="1:31" ht="15" customHeight="1">
       <c r="A43" s="76" t="s">
@@ -6182,11 +6218,11 @@
       <c r="AE46" s="110"/>
     </row>
     <row r="47" spans="1:31" s="64" customFormat="1" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A47" s="192" t="s">
+      <c r="A47" s="171" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="193"/>
-      <c r="C47" s="194"/>
+      <c r="B47" s="172"/>
+      <c r="C47" s="173"/>
       <c r="D47" s="228" t="s">
         <v>149</v>
       </c>
@@ -6245,11 +6281,11 @@
       <c r="AE47" s="213"/>
     </row>
     <row r="48" spans="1:31" s="4" customFormat="1" ht="20" customHeight="1">
-      <c r="A48" s="195" t="s">
+      <c r="A48" s="174" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="196"/>
-      <c r="C48" s="197"/>
+      <c r="B48" s="175"/>
+      <c r="C48" s="176"/>
       <c r="D48" s="209" t="s">
         <v>111</v>
       </c>
@@ -6282,48 +6318,48 @@
       <c r="AE48" s="210"/>
     </row>
     <row r="49" spans="1:31" s="4" customFormat="1" ht="20" customHeight="1">
-      <c r="A49" s="183" t="s">
+      <c r="A49" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="184"/>
-      <c r="C49" s="185"/>
-      <c r="D49" s="171" t="s">
+      <c r="B49" s="178"/>
+      <c r="C49" s="179"/>
+      <c r="D49" s="184" t="s">
         <v>110</v>
       </c>
-      <c r="E49" s="171"/>
-      <c r="F49" s="171"/>
-      <c r="G49" s="171"/>
-      <c r="H49" s="171"/>
-      <c r="I49" s="171"/>
-      <c r="J49" s="171"/>
-      <c r="K49" s="171"/>
-      <c r="L49" s="171"/>
-      <c r="M49" s="171"/>
-      <c r="N49" s="171"/>
-      <c r="O49" s="171"/>
-      <c r="P49" s="171"/>
-      <c r="Q49" s="171"/>
-      <c r="R49" s="171"/>
-      <c r="S49" s="171"/>
-      <c r="T49" s="171"/>
-      <c r="U49" s="171"/>
-      <c r="V49" s="171"/>
-      <c r="W49" s="171"/>
-      <c r="X49" s="171"/>
-      <c r="Y49" s="171"/>
-      <c r="Z49" s="171"/>
-      <c r="AA49" s="171"/>
-      <c r="AB49" s="171"/>
-      <c r="AC49" s="171"/>
-      <c r="AD49" s="171"/>
+      <c r="E49" s="184"/>
+      <c r="F49" s="184"/>
+      <c r="G49" s="184"/>
+      <c r="H49" s="184"/>
+      <c r="I49" s="184"/>
+      <c r="J49" s="184"/>
+      <c r="K49" s="184"/>
+      <c r="L49" s="184"/>
+      <c r="M49" s="184"/>
+      <c r="N49" s="184"/>
+      <c r="O49" s="184"/>
+      <c r="P49" s="184"/>
+      <c r="Q49" s="184"/>
+      <c r="R49" s="184"/>
+      <c r="S49" s="184"/>
+      <c r="T49" s="184"/>
+      <c r="U49" s="184"/>
+      <c r="V49" s="184"/>
+      <c r="W49" s="184"/>
+      <c r="X49" s="184"/>
+      <c r="Y49" s="184"/>
+      <c r="Z49" s="184"/>
+      <c r="AA49" s="184"/>
+      <c r="AB49" s="184"/>
+      <c r="AC49" s="184"/>
+      <c r="AD49" s="184"/>
       <c r="AE49" s="208"/>
     </row>
     <row r="50" spans="1:31" s="4" customFormat="1" ht="20" customHeight="1">
-      <c r="A50" s="183" t="s">
+      <c r="A50" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="184"/>
-      <c r="C50" s="185"/>
+      <c r="B50" s="178"/>
+      <c r="C50" s="179"/>
       <c r="D50" s="67"/>
       <c r="E50" s="68"/>
       <c r="F50" s="67"/>
@@ -6354,11 +6390,11 @@
       <c r="AE50" s="85"/>
     </row>
     <row r="51" spans="1:31" s="4" customFormat="1" ht="20" customHeight="1">
-      <c r="A51" s="183" t="s">
+      <c r="A51" s="177" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="184"/>
-      <c r="C51" s="185"/>
+      <c r="B51" s="178"/>
+      <c r="C51" s="179"/>
       <c r="D51" s="220"/>
       <c r="E51" s="220"/>
       <c r="F51" s="206"/>
@@ -6389,13 +6425,13 @@
       <c r="AE51" s="207"/>
     </row>
     <row r="52" spans="1:31" s="4" customFormat="1" ht="20" customHeight="1">
-      <c r="A52" s="183" t="s">
+      <c r="A52" s="177" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="184"/>
-      <c r="C52" s="185"/>
-      <c r="D52" s="171"/>
-      <c r="E52" s="171"/>
+      <c r="B52" s="178"/>
+      <c r="C52" s="179"/>
+      <c r="D52" s="184"/>
+      <c r="E52" s="184"/>
       <c r="F52" s="206"/>
       <c r="G52" s="206"/>
       <c r="H52" s="206"/>
@@ -6424,115 +6460,115 @@
       <c r="AE52" s="207"/>
     </row>
     <row r="53" spans="1:31" s="4" customFormat="1" ht="20" customHeight="1">
-      <c r="A53" s="183" t="s">
+      <c r="A53" s="177" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="184"/>
-      <c r="C53" s="185"/>
-      <c r="D53" s="171" t="s">
+      <c r="B53" s="178"/>
+      <c r="C53" s="179"/>
+      <c r="D53" s="184" t="s">
         <v>100</v>
       </c>
-      <c r="E53" s="171"/>
-      <c r="F53" s="171"/>
-      <c r="G53" s="171"/>
-      <c r="H53" s="171"/>
-      <c r="I53" s="171"/>
-      <c r="J53" s="171"/>
-      <c r="K53" s="171"/>
-      <c r="L53" s="171"/>
-      <c r="M53" s="171"/>
-      <c r="N53" s="171"/>
-      <c r="O53" s="171"/>
-      <c r="P53" s="171"/>
-      <c r="Q53" s="171"/>
-      <c r="R53" s="171"/>
-      <c r="S53" s="171"/>
-      <c r="T53" s="171"/>
-      <c r="U53" s="171"/>
-      <c r="V53" s="171"/>
-      <c r="W53" s="171"/>
-      <c r="X53" s="171"/>
-      <c r="Y53" s="171"/>
-      <c r="Z53" s="171"/>
-      <c r="AA53" s="171"/>
-      <c r="AB53" s="171"/>
-      <c r="AC53" s="171"/>
-      <c r="AD53" s="171"/>
-      <c r="AE53" s="171"/>
+      <c r="E53" s="184"/>
+      <c r="F53" s="184"/>
+      <c r="G53" s="184"/>
+      <c r="H53" s="184"/>
+      <c r="I53" s="184"/>
+      <c r="J53" s="184"/>
+      <c r="K53" s="184"/>
+      <c r="L53" s="184"/>
+      <c r="M53" s="184"/>
+      <c r="N53" s="184"/>
+      <c r="O53" s="184"/>
+      <c r="P53" s="184"/>
+      <c r="Q53" s="184"/>
+      <c r="R53" s="184"/>
+      <c r="S53" s="184"/>
+      <c r="T53" s="184"/>
+      <c r="U53" s="184"/>
+      <c r="V53" s="184"/>
+      <c r="W53" s="184"/>
+      <c r="X53" s="184"/>
+      <c r="Y53" s="184"/>
+      <c r="Z53" s="184"/>
+      <c r="AA53" s="184"/>
+      <c r="AB53" s="184"/>
+      <c r="AC53" s="184"/>
+      <c r="AD53" s="184"/>
+      <c r="AE53" s="184"/>
     </row>
     <row r="54" spans="1:31" s="4" customFormat="1" ht="20" customHeight="1" thickBot="1">
-      <c r="A54" s="186" t="s">
+      <c r="A54" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="187"/>
-      <c r="C54" s="188"/>
-      <c r="D54" s="204" t="s">
+      <c r="B54" s="198"/>
+      <c r="C54" s="199"/>
+      <c r="D54" s="186" t="s">
         <v>112</v>
       </c>
-      <c r="E54" s="204"/>
-      <c r="F54" s="204"/>
-      <c r="G54" s="204"/>
-      <c r="H54" s="204"/>
-      <c r="I54" s="204"/>
-      <c r="J54" s="204"/>
-      <c r="K54" s="204"/>
-      <c r="L54" s="204"/>
-      <c r="M54" s="204"/>
-      <c r="N54" s="204"/>
-      <c r="O54" s="204"/>
-      <c r="P54" s="204"/>
-      <c r="Q54" s="204"/>
-      <c r="R54" s="204"/>
-      <c r="S54" s="204"/>
-      <c r="T54" s="204"/>
-      <c r="U54" s="204"/>
-      <c r="V54" s="204"/>
-      <c r="W54" s="204"/>
-      <c r="X54" s="204"/>
-      <c r="Y54" s="204"/>
-      <c r="Z54" s="204"/>
-      <c r="AA54" s="204"/>
-      <c r="AB54" s="204"/>
-      <c r="AC54" s="204"/>
-      <c r="AD54" s="204"/>
-      <c r="AE54" s="205"/>
+      <c r="E54" s="186"/>
+      <c r="F54" s="186"/>
+      <c r="G54" s="186"/>
+      <c r="H54" s="186"/>
+      <c r="I54" s="186"/>
+      <c r="J54" s="186"/>
+      <c r="K54" s="186"/>
+      <c r="L54" s="186"/>
+      <c r="M54" s="186"/>
+      <c r="N54" s="186"/>
+      <c r="O54" s="186"/>
+      <c r="P54" s="186"/>
+      <c r="Q54" s="186"/>
+      <c r="R54" s="186"/>
+      <c r="S54" s="186"/>
+      <c r="T54" s="186"/>
+      <c r="U54" s="186"/>
+      <c r="V54" s="186"/>
+      <c r="W54" s="186"/>
+      <c r="X54" s="186"/>
+      <c r="Y54" s="186"/>
+      <c r="Z54" s="186"/>
+      <c r="AA54" s="186"/>
+      <c r="AB54" s="186"/>
+      <c r="AC54" s="186"/>
+      <c r="AD54" s="186"/>
+      <c r="AE54" s="187"/>
     </row>
     <row r="55" spans="1:31" s="4" customFormat="1" ht="20" customHeight="1" thickBot="1">
-      <c r="A55" s="189" t="s">
+      <c r="A55" s="200" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="190"/>
-      <c r="C55" s="191"/>
-      <c r="D55" s="204" t="s">
+      <c r="B55" s="201"/>
+      <c r="C55" s="202"/>
+      <c r="D55" s="186" t="s">
         <v>117</v>
       </c>
-      <c r="E55" s="204"/>
-      <c r="F55" s="204"/>
-      <c r="G55" s="204"/>
-      <c r="H55" s="204"/>
-      <c r="I55" s="204"/>
-      <c r="J55" s="204"/>
-      <c r="K55" s="204"/>
-      <c r="L55" s="204"/>
-      <c r="M55" s="204"/>
-      <c r="N55" s="204"/>
-      <c r="O55" s="204"/>
+      <c r="E55" s="186"/>
+      <c r="F55" s="186"/>
+      <c r="G55" s="186"/>
+      <c r="H55" s="186"/>
+      <c r="I55" s="186"/>
+      <c r="J55" s="186"/>
+      <c r="K55" s="186"/>
+      <c r="L55" s="186"/>
+      <c r="M55" s="186"/>
+      <c r="N55" s="186"/>
+      <c r="O55" s="186"/>
       <c r="P55" s="130"/>
       <c r="Q55" s="130"/>
-      <c r="R55" s="204"/>
-      <c r="S55" s="204"/>
+      <c r="R55" s="186"/>
+      <c r="S55" s="186"/>
       <c r="T55" s="130"/>
       <c r="U55" s="130"/>
-      <c r="V55" s="204"/>
-      <c r="W55" s="204"/>
+      <c r="V55" s="186"/>
+      <c r="W55" s="186"/>
       <c r="X55" s="130"/>
       <c r="Y55" s="130"/>
-      <c r="Z55" s="204"/>
-      <c r="AA55" s="204"/>
+      <c r="Z55" s="186"/>
+      <c r="AA55" s="186"/>
       <c r="AB55" s="130"/>
       <c r="AC55" s="130"/>
-      <c r="AD55" s="204"/>
-      <c r="AE55" s="205"/>
+      <c r="AD55" s="186"/>
+      <c r="AE55" s="187"/>
     </row>
     <row r="56" spans="1:31" s="7" customFormat="1" ht="6.75" customHeight="1">
       <c r="A56" s="131"/>
@@ -6603,9 +6639,9 @@
       <c r="AE57" s="131"/>
     </row>
     <row r="58" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A58" s="172"/>
-      <c r="B58" s="173"/>
-      <c r="C58" s="176"/>
+      <c r="A58" s="188"/>
+      <c r="B58" s="189"/>
+      <c r="C58" s="190"/>
       <c r="D58" s="218"/>
       <c r="E58" s="214"/>
       <c r="F58" s="214"/>
@@ -6636,108 +6672,108 @@
       <c r="AE58" s="214"/>
     </row>
     <row r="59" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A59" s="177"/>
-      <c r="B59" s="178"/>
-      <c r="C59" s="179"/>
+      <c r="A59" s="191"/>
+      <c r="B59" s="192"/>
+      <c r="C59" s="193"/>
       <c r="D59" s="217"/>
-      <c r="E59" s="203"/>
-      <c r="F59" s="203"/>
-      <c r="G59" s="203"/>
-      <c r="H59" s="203"/>
-      <c r="I59" s="203"/>
-      <c r="J59" s="203"/>
-      <c r="K59" s="203"/>
-      <c r="L59" s="203"/>
-      <c r="M59" s="203"/>
-      <c r="N59" s="203"/>
-      <c r="O59" s="203"/>
-      <c r="P59" s="203"/>
-      <c r="Q59" s="203"/>
-      <c r="R59" s="203"/>
-      <c r="S59" s="203"/>
-      <c r="T59" s="203"/>
-      <c r="U59" s="203"/>
-      <c r="V59" s="203"/>
-      <c r="W59" s="203"/>
-      <c r="X59" s="203"/>
-      <c r="Y59" s="203"/>
-      <c r="Z59" s="203"/>
-      <c r="AA59" s="203"/>
-      <c r="AB59" s="203"/>
-      <c r="AC59" s="203"/>
-      <c r="AD59" s="203"/>
-      <c r="AE59" s="203"/>
+      <c r="E59" s="185"/>
+      <c r="F59" s="185"/>
+      <c r="G59" s="185"/>
+      <c r="H59" s="185"/>
+      <c r="I59" s="185"/>
+      <c r="J59" s="185"/>
+      <c r="K59" s="185"/>
+      <c r="L59" s="185"/>
+      <c r="M59" s="185"/>
+      <c r="N59" s="185"/>
+      <c r="O59" s="185"/>
+      <c r="P59" s="185"/>
+      <c r="Q59" s="185"/>
+      <c r="R59" s="185"/>
+      <c r="S59" s="185"/>
+      <c r="T59" s="185"/>
+      <c r="U59" s="185"/>
+      <c r="V59" s="185"/>
+      <c r="W59" s="185"/>
+      <c r="X59" s="185"/>
+      <c r="Y59" s="185"/>
+      <c r="Z59" s="185"/>
+      <c r="AA59" s="185"/>
+      <c r="AB59" s="185"/>
+      <c r="AC59" s="185"/>
+      <c r="AD59" s="185"/>
+      <c r="AE59" s="185"/>
     </row>
     <row r="60" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A60" s="177"/>
-      <c r="B60" s="178"/>
-      <c r="C60" s="179"/>
+      <c r="A60" s="191"/>
+      <c r="B60" s="192"/>
+      <c r="C60" s="193"/>
       <c r="D60" s="217"/>
-      <c r="E60" s="203"/>
-      <c r="F60" s="203"/>
-      <c r="G60" s="203"/>
-      <c r="H60" s="203"/>
-      <c r="I60" s="203"/>
-      <c r="J60" s="203"/>
-      <c r="K60" s="203"/>
-      <c r="L60" s="203"/>
-      <c r="M60" s="203"/>
-      <c r="N60" s="203"/>
-      <c r="O60" s="203"/>
-      <c r="P60" s="203"/>
-      <c r="Q60" s="203"/>
-      <c r="R60" s="203"/>
-      <c r="S60" s="203"/>
-      <c r="T60" s="203"/>
-      <c r="U60" s="203"/>
-      <c r="V60" s="203"/>
-      <c r="W60" s="203"/>
-      <c r="X60" s="203"/>
-      <c r="Y60" s="203"/>
-      <c r="Z60" s="203"/>
-      <c r="AA60" s="203"/>
-      <c r="AB60" s="203"/>
-      <c r="AC60" s="203"/>
-      <c r="AD60" s="203"/>
-      <c r="AE60" s="203"/>
+      <c r="E60" s="185"/>
+      <c r="F60" s="185"/>
+      <c r="G60" s="185"/>
+      <c r="H60" s="185"/>
+      <c r="I60" s="185"/>
+      <c r="J60" s="185"/>
+      <c r="K60" s="185"/>
+      <c r="L60" s="185"/>
+      <c r="M60" s="185"/>
+      <c r="N60" s="185"/>
+      <c r="O60" s="185"/>
+      <c r="P60" s="185"/>
+      <c r="Q60" s="185"/>
+      <c r="R60" s="185"/>
+      <c r="S60" s="185"/>
+      <c r="T60" s="185"/>
+      <c r="U60" s="185"/>
+      <c r="V60" s="185"/>
+      <c r="W60" s="185"/>
+      <c r="X60" s="185"/>
+      <c r="Y60" s="185"/>
+      <c r="Z60" s="185"/>
+      <c r="AA60" s="185"/>
+      <c r="AB60" s="185"/>
+      <c r="AC60" s="185"/>
+      <c r="AD60" s="185"/>
+      <c r="AE60" s="185"/>
     </row>
     <row r="61" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A61" s="177"/>
-      <c r="B61" s="178"/>
-      <c r="C61" s="179"/>
+      <c r="A61" s="191"/>
+      <c r="B61" s="192"/>
+      <c r="C61" s="193"/>
       <c r="D61" s="217"/>
-      <c r="E61" s="203"/>
-      <c r="F61" s="203"/>
-      <c r="G61" s="203"/>
-      <c r="H61" s="203"/>
-      <c r="I61" s="203"/>
-      <c r="J61" s="203"/>
-      <c r="K61" s="203"/>
-      <c r="L61" s="203"/>
-      <c r="M61" s="203"/>
-      <c r="N61" s="203"/>
-      <c r="O61" s="203"/>
-      <c r="P61" s="203"/>
-      <c r="Q61" s="203"/>
-      <c r="R61" s="203"/>
-      <c r="S61" s="203"/>
-      <c r="T61" s="203"/>
-      <c r="U61" s="203"/>
-      <c r="V61" s="203"/>
-      <c r="W61" s="203"/>
-      <c r="X61" s="203"/>
-      <c r="Y61" s="203"/>
-      <c r="Z61" s="203"/>
-      <c r="AA61" s="203"/>
-      <c r="AB61" s="203"/>
-      <c r="AC61" s="203"/>
-      <c r="AD61" s="203"/>
-      <c r="AE61" s="203"/>
+      <c r="E61" s="185"/>
+      <c r="F61" s="185"/>
+      <c r="G61" s="185"/>
+      <c r="H61" s="185"/>
+      <c r="I61" s="185"/>
+      <c r="J61" s="185"/>
+      <c r="K61" s="185"/>
+      <c r="L61" s="185"/>
+      <c r="M61" s="185"/>
+      <c r="N61" s="185"/>
+      <c r="O61" s="185"/>
+      <c r="P61" s="185"/>
+      <c r="Q61" s="185"/>
+      <c r="R61" s="185"/>
+      <c r="S61" s="185"/>
+      <c r="T61" s="185"/>
+      <c r="U61" s="185"/>
+      <c r="V61" s="185"/>
+      <c r="W61" s="185"/>
+      <c r="X61" s="185"/>
+      <c r="Y61" s="185"/>
+      <c r="Z61" s="185"/>
+      <c r="AA61" s="185"/>
+      <c r="AB61" s="185"/>
+      <c r="AC61" s="185"/>
+      <c r="AD61" s="185"/>
+      <c r="AE61" s="185"/>
     </row>
     <row r="62" spans="1:31" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A62" s="180"/>
-      <c r="B62" s="181"/>
-      <c r="C62" s="182"/>
+      <c r="A62" s="194"/>
+      <c r="B62" s="195"/>
+      <c r="C62" s="196"/>
       <c r="D62" s="219"/>
       <c r="E62" s="216"/>
       <c r="F62" s="216"/>
@@ -6768,9 +6804,9 @@
       <c r="AE62" s="216"/>
     </row>
     <row r="63" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A63" s="172"/>
-      <c r="B63" s="173"/>
-      <c r="C63" s="176"/>
+      <c r="A63" s="188"/>
+      <c r="B63" s="189"/>
+      <c r="C63" s="190"/>
       <c r="D63" s="218"/>
       <c r="E63" s="214"/>
       <c r="F63" s="214"/>
@@ -6801,108 +6837,108 @@
       <c r="AE63" s="214"/>
     </row>
     <row r="64" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A64" s="177"/>
-      <c r="B64" s="178"/>
-      <c r="C64" s="179"/>
+      <c r="A64" s="191"/>
+      <c r="B64" s="192"/>
+      <c r="C64" s="193"/>
       <c r="D64" s="217"/>
-      <c r="E64" s="203"/>
-      <c r="F64" s="203"/>
-      <c r="G64" s="203"/>
-      <c r="H64" s="203"/>
-      <c r="I64" s="203"/>
-      <c r="J64" s="203"/>
-      <c r="K64" s="203"/>
-      <c r="L64" s="203"/>
-      <c r="M64" s="203"/>
-      <c r="N64" s="203"/>
-      <c r="O64" s="203"/>
-      <c r="P64" s="203"/>
-      <c r="Q64" s="203"/>
-      <c r="R64" s="203"/>
-      <c r="S64" s="203"/>
-      <c r="T64" s="203"/>
-      <c r="U64" s="203"/>
-      <c r="V64" s="203"/>
-      <c r="W64" s="203"/>
-      <c r="X64" s="203"/>
-      <c r="Y64" s="203"/>
-      <c r="Z64" s="203"/>
-      <c r="AA64" s="203"/>
-      <c r="AB64" s="203"/>
-      <c r="AC64" s="203"/>
-      <c r="AD64" s="203"/>
-      <c r="AE64" s="203"/>
+      <c r="E64" s="185"/>
+      <c r="F64" s="185"/>
+      <c r="G64" s="185"/>
+      <c r="H64" s="185"/>
+      <c r="I64" s="185"/>
+      <c r="J64" s="185"/>
+      <c r="K64" s="185"/>
+      <c r="L64" s="185"/>
+      <c r="M64" s="185"/>
+      <c r="N64" s="185"/>
+      <c r="O64" s="185"/>
+      <c r="P64" s="185"/>
+      <c r="Q64" s="185"/>
+      <c r="R64" s="185"/>
+      <c r="S64" s="185"/>
+      <c r="T64" s="185"/>
+      <c r="U64" s="185"/>
+      <c r="V64" s="185"/>
+      <c r="W64" s="185"/>
+      <c r="X64" s="185"/>
+      <c r="Y64" s="185"/>
+      <c r="Z64" s="185"/>
+      <c r="AA64" s="185"/>
+      <c r="AB64" s="185"/>
+      <c r="AC64" s="185"/>
+      <c r="AD64" s="185"/>
+      <c r="AE64" s="185"/>
     </row>
     <row r="65" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A65" s="177"/>
-      <c r="B65" s="178"/>
-      <c r="C65" s="179"/>
+      <c r="A65" s="191"/>
+      <c r="B65" s="192"/>
+      <c r="C65" s="193"/>
       <c r="D65" s="217"/>
-      <c r="E65" s="203"/>
-      <c r="F65" s="203"/>
-      <c r="G65" s="203"/>
-      <c r="H65" s="203"/>
-      <c r="I65" s="203"/>
-      <c r="J65" s="203"/>
-      <c r="K65" s="203"/>
-      <c r="L65" s="203"/>
-      <c r="M65" s="203"/>
-      <c r="N65" s="203"/>
-      <c r="O65" s="203"/>
-      <c r="P65" s="203"/>
-      <c r="Q65" s="203"/>
-      <c r="R65" s="203"/>
-      <c r="S65" s="203"/>
-      <c r="T65" s="203"/>
-      <c r="U65" s="203"/>
-      <c r="V65" s="203"/>
-      <c r="W65" s="203"/>
-      <c r="X65" s="203"/>
-      <c r="Y65" s="203"/>
-      <c r="Z65" s="203"/>
-      <c r="AA65" s="203"/>
-      <c r="AB65" s="203"/>
-      <c r="AC65" s="203"/>
-      <c r="AD65" s="203"/>
-      <c r="AE65" s="203"/>
+      <c r="E65" s="185"/>
+      <c r="F65" s="185"/>
+      <c r="G65" s="185"/>
+      <c r="H65" s="185"/>
+      <c r="I65" s="185"/>
+      <c r="J65" s="185"/>
+      <c r="K65" s="185"/>
+      <c r="L65" s="185"/>
+      <c r="M65" s="185"/>
+      <c r="N65" s="185"/>
+      <c r="O65" s="185"/>
+      <c r="P65" s="185"/>
+      <c r="Q65" s="185"/>
+      <c r="R65" s="185"/>
+      <c r="S65" s="185"/>
+      <c r="T65" s="185"/>
+      <c r="U65" s="185"/>
+      <c r="V65" s="185"/>
+      <c r="W65" s="185"/>
+      <c r="X65" s="185"/>
+      <c r="Y65" s="185"/>
+      <c r="Z65" s="185"/>
+      <c r="AA65" s="185"/>
+      <c r="AB65" s="185"/>
+      <c r="AC65" s="185"/>
+      <c r="AD65" s="185"/>
+      <c r="AE65" s="185"/>
     </row>
     <row r="66" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A66" s="177"/>
-      <c r="B66" s="178"/>
-      <c r="C66" s="179"/>
+      <c r="A66" s="191"/>
+      <c r="B66" s="192"/>
+      <c r="C66" s="193"/>
       <c r="D66" s="217"/>
-      <c r="E66" s="203"/>
-      <c r="F66" s="203"/>
-      <c r="G66" s="203"/>
-      <c r="H66" s="203"/>
-      <c r="I66" s="203"/>
-      <c r="J66" s="203"/>
-      <c r="K66" s="203"/>
-      <c r="L66" s="203"/>
-      <c r="M66" s="203"/>
-      <c r="N66" s="203"/>
-      <c r="O66" s="203"/>
-      <c r="P66" s="203"/>
-      <c r="Q66" s="203"/>
-      <c r="R66" s="203"/>
-      <c r="S66" s="203"/>
-      <c r="T66" s="203"/>
-      <c r="U66" s="203"/>
-      <c r="V66" s="203"/>
-      <c r="W66" s="203"/>
-      <c r="X66" s="203"/>
-      <c r="Y66" s="203"/>
-      <c r="Z66" s="203"/>
-      <c r="AA66" s="203"/>
-      <c r="AB66" s="203"/>
-      <c r="AC66" s="203"/>
-      <c r="AD66" s="203"/>
-      <c r="AE66" s="203"/>
+      <c r="E66" s="185"/>
+      <c r="F66" s="185"/>
+      <c r="G66" s="185"/>
+      <c r="H66" s="185"/>
+      <c r="I66" s="185"/>
+      <c r="J66" s="185"/>
+      <c r="K66" s="185"/>
+      <c r="L66" s="185"/>
+      <c r="M66" s="185"/>
+      <c r="N66" s="185"/>
+      <c r="O66" s="185"/>
+      <c r="P66" s="185"/>
+      <c r="Q66" s="185"/>
+      <c r="R66" s="185"/>
+      <c r="S66" s="185"/>
+      <c r="T66" s="185"/>
+      <c r="U66" s="185"/>
+      <c r="V66" s="185"/>
+      <c r="W66" s="185"/>
+      <c r="X66" s="185"/>
+      <c r="Y66" s="185"/>
+      <c r="Z66" s="185"/>
+      <c r="AA66" s="185"/>
+      <c r="AB66" s="185"/>
+      <c r="AC66" s="185"/>
+      <c r="AD66" s="185"/>
+      <c r="AE66" s="185"/>
     </row>
     <row r="67" spans="1:31" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A67" s="180"/>
-      <c r="B67" s="181"/>
-      <c r="C67" s="182"/>
+      <c r="A67" s="194"/>
+      <c r="B67" s="195"/>
+      <c r="C67" s="196"/>
       <c r="D67" s="219"/>
       <c r="E67" s="216"/>
       <c r="F67" s="216"/>
@@ -6933,9 +6969,9 @@
       <c r="AE67" s="216"/>
     </row>
     <row r="68" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A68" s="172"/>
-      <c r="B68" s="173"/>
-      <c r="C68" s="176"/>
+      <c r="A68" s="188"/>
+      <c r="B68" s="189"/>
+      <c r="C68" s="190"/>
       <c r="D68" s="218"/>
       <c r="E68" s="214"/>
       <c r="F68" s="214"/>
@@ -6966,108 +7002,108 @@
       <c r="AE68" s="214"/>
     </row>
     <row r="69" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A69" s="177"/>
-      <c r="B69" s="178"/>
-      <c r="C69" s="179"/>
+      <c r="A69" s="191"/>
+      <c r="B69" s="192"/>
+      <c r="C69" s="193"/>
       <c r="D69" s="217"/>
-      <c r="E69" s="203"/>
-      <c r="F69" s="203"/>
-      <c r="G69" s="203"/>
-      <c r="H69" s="203"/>
-      <c r="I69" s="203"/>
-      <c r="J69" s="203"/>
-      <c r="K69" s="203"/>
-      <c r="L69" s="203"/>
-      <c r="M69" s="203"/>
-      <c r="N69" s="203"/>
-      <c r="O69" s="203"/>
-      <c r="P69" s="203"/>
-      <c r="Q69" s="203"/>
-      <c r="R69" s="203"/>
-      <c r="S69" s="203"/>
-      <c r="T69" s="203"/>
-      <c r="U69" s="203"/>
-      <c r="V69" s="203"/>
-      <c r="W69" s="203"/>
-      <c r="X69" s="203"/>
-      <c r="Y69" s="203"/>
-      <c r="Z69" s="203"/>
-      <c r="AA69" s="203"/>
-      <c r="AB69" s="203"/>
-      <c r="AC69" s="203"/>
-      <c r="AD69" s="203"/>
-      <c r="AE69" s="203"/>
+      <c r="E69" s="185"/>
+      <c r="F69" s="185"/>
+      <c r="G69" s="185"/>
+      <c r="H69" s="185"/>
+      <c r="I69" s="185"/>
+      <c r="J69" s="185"/>
+      <c r="K69" s="185"/>
+      <c r="L69" s="185"/>
+      <c r="M69" s="185"/>
+      <c r="N69" s="185"/>
+      <c r="O69" s="185"/>
+      <c r="P69" s="185"/>
+      <c r="Q69" s="185"/>
+      <c r="R69" s="185"/>
+      <c r="S69" s="185"/>
+      <c r="T69" s="185"/>
+      <c r="U69" s="185"/>
+      <c r="V69" s="185"/>
+      <c r="W69" s="185"/>
+      <c r="X69" s="185"/>
+      <c r="Y69" s="185"/>
+      <c r="Z69" s="185"/>
+      <c r="AA69" s="185"/>
+      <c r="AB69" s="185"/>
+      <c r="AC69" s="185"/>
+      <c r="AD69" s="185"/>
+      <c r="AE69" s="185"/>
     </row>
     <row r="70" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A70" s="177"/>
-      <c r="B70" s="178"/>
-      <c r="C70" s="179"/>
+      <c r="A70" s="191"/>
+      <c r="B70" s="192"/>
+      <c r="C70" s="193"/>
       <c r="D70" s="217"/>
-      <c r="E70" s="203"/>
-      <c r="F70" s="203"/>
-      <c r="G70" s="203"/>
-      <c r="H70" s="203"/>
-      <c r="I70" s="203"/>
-      <c r="J70" s="203"/>
-      <c r="K70" s="203"/>
-      <c r="L70" s="203"/>
-      <c r="M70" s="203"/>
-      <c r="N70" s="203"/>
-      <c r="O70" s="203"/>
-      <c r="P70" s="203"/>
-      <c r="Q70" s="203"/>
-      <c r="R70" s="203"/>
-      <c r="S70" s="203"/>
-      <c r="T70" s="203"/>
-      <c r="U70" s="203"/>
-      <c r="V70" s="203"/>
-      <c r="W70" s="203"/>
-      <c r="X70" s="203"/>
-      <c r="Y70" s="203"/>
-      <c r="Z70" s="203"/>
-      <c r="AA70" s="203"/>
-      <c r="AB70" s="203"/>
-      <c r="AC70" s="203"/>
-      <c r="AD70" s="203"/>
-      <c r="AE70" s="203"/>
+      <c r="E70" s="185"/>
+      <c r="F70" s="185"/>
+      <c r="G70" s="185"/>
+      <c r="H70" s="185"/>
+      <c r="I70" s="185"/>
+      <c r="J70" s="185"/>
+      <c r="K70" s="185"/>
+      <c r="L70" s="185"/>
+      <c r="M70" s="185"/>
+      <c r="N70" s="185"/>
+      <c r="O70" s="185"/>
+      <c r="P70" s="185"/>
+      <c r="Q70" s="185"/>
+      <c r="R70" s="185"/>
+      <c r="S70" s="185"/>
+      <c r="T70" s="185"/>
+      <c r="U70" s="185"/>
+      <c r="V70" s="185"/>
+      <c r="W70" s="185"/>
+      <c r="X70" s="185"/>
+      <c r="Y70" s="185"/>
+      <c r="Z70" s="185"/>
+      <c r="AA70" s="185"/>
+      <c r="AB70" s="185"/>
+      <c r="AC70" s="185"/>
+      <c r="AD70" s="185"/>
+      <c r="AE70" s="185"/>
     </row>
     <row r="71" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A71" s="177"/>
-      <c r="B71" s="178"/>
-      <c r="C71" s="179"/>
+      <c r="A71" s="191"/>
+      <c r="B71" s="192"/>
+      <c r="C71" s="193"/>
       <c r="D71" s="217"/>
-      <c r="E71" s="203"/>
-      <c r="F71" s="203"/>
-      <c r="G71" s="203"/>
-      <c r="H71" s="203"/>
-      <c r="I71" s="203"/>
-      <c r="J71" s="203"/>
-      <c r="K71" s="203"/>
-      <c r="L71" s="203"/>
-      <c r="M71" s="203"/>
-      <c r="N71" s="203"/>
-      <c r="O71" s="203"/>
-      <c r="P71" s="203"/>
-      <c r="Q71" s="203"/>
-      <c r="R71" s="203"/>
-      <c r="S71" s="203"/>
-      <c r="T71" s="203"/>
-      <c r="U71" s="203"/>
-      <c r="V71" s="203"/>
-      <c r="W71" s="203"/>
-      <c r="X71" s="203"/>
-      <c r="Y71" s="203"/>
-      <c r="Z71" s="203"/>
-      <c r="AA71" s="203"/>
-      <c r="AB71" s="203"/>
-      <c r="AC71" s="203"/>
-      <c r="AD71" s="203"/>
-      <c r="AE71" s="203"/>
+      <c r="E71" s="185"/>
+      <c r="F71" s="185"/>
+      <c r="G71" s="185"/>
+      <c r="H71" s="185"/>
+      <c r="I71" s="185"/>
+      <c r="J71" s="185"/>
+      <c r="K71" s="185"/>
+      <c r="L71" s="185"/>
+      <c r="M71" s="185"/>
+      <c r="N71" s="185"/>
+      <c r="O71" s="185"/>
+      <c r="P71" s="185"/>
+      <c r="Q71" s="185"/>
+      <c r="R71" s="185"/>
+      <c r="S71" s="185"/>
+      <c r="T71" s="185"/>
+      <c r="U71" s="185"/>
+      <c r="V71" s="185"/>
+      <c r="W71" s="185"/>
+      <c r="X71" s="185"/>
+      <c r="Y71" s="185"/>
+      <c r="Z71" s="185"/>
+      <c r="AA71" s="185"/>
+      <c r="AB71" s="185"/>
+      <c r="AC71" s="185"/>
+      <c r="AD71" s="185"/>
+      <c r="AE71" s="185"/>
     </row>
     <row r="72" spans="1:31" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A72" s="180"/>
-      <c r="B72" s="181"/>
-      <c r="C72" s="182"/>
+      <c r="A72" s="194"/>
+      <c r="B72" s="195"/>
+      <c r="C72" s="196"/>
       <c r="D72" s="219"/>
       <c r="E72" s="216"/>
       <c r="F72" s="216"/>
@@ -7098,9 +7134,9 @@
       <c r="AE72" s="216"/>
     </row>
     <row r="73" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A73" s="172"/>
-      <c r="B73" s="173"/>
-      <c r="C73" s="176"/>
+      <c r="A73" s="188"/>
+      <c r="B73" s="189"/>
+      <c r="C73" s="190"/>
       <c r="D73" s="218"/>
       <c r="E73" s="214"/>
       <c r="F73" s="214"/>
@@ -7131,108 +7167,108 @@
       <c r="AE73" s="214"/>
     </row>
     <row r="74" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A74" s="177"/>
-      <c r="B74" s="178"/>
-      <c r="C74" s="179"/>
+      <c r="A74" s="191"/>
+      <c r="B74" s="192"/>
+      <c r="C74" s="193"/>
       <c r="D74" s="217"/>
-      <c r="E74" s="203"/>
-      <c r="F74" s="203"/>
-      <c r="G74" s="203"/>
-      <c r="H74" s="203"/>
-      <c r="I74" s="203"/>
-      <c r="J74" s="203"/>
-      <c r="K74" s="203"/>
-      <c r="L74" s="203"/>
-      <c r="M74" s="203"/>
-      <c r="N74" s="203"/>
-      <c r="O74" s="203"/>
-      <c r="P74" s="203"/>
-      <c r="Q74" s="203"/>
-      <c r="R74" s="203"/>
-      <c r="S74" s="203"/>
-      <c r="T74" s="203"/>
-      <c r="U74" s="203"/>
-      <c r="V74" s="203"/>
-      <c r="W74" s="203"/>
-      <c r="X74" s="203"/>
-      <c r="Y74" s="203"/>
-      <c r="Z74" s="203"/>
-      <c r="AA74" s="203"/>
-      <c r="AB74" s="203"/>
-      <c r="AC74" s="203"/>
-      <c r="AD74" s="203"/>
-      <c r="AE74" s="203"/>
+      <c r="E74" s="185"/>
+      <c r="F74" s="185"/>
+      <c r="G74" s="185"/>
+      <c r="H74" s="185"/>
+      <c r="I74" s="185"/>
+      <c r="J74" s="185"/>
+      <c r="K74" s="185"/>
+      <c r="L74" s="185"/>
+      <c r="M74" s="185"/>
+      <c r="N74" s="185"/>
+      <c r="O74" s="185"/>
+      <c r="P74" s="185"/>
+      <c r="Q74" s="185"/>
+      <c r="R74" s="185"/>
+      <c r="S74" s="185"/>
+      <c r="T74" s="185"/>
+      <c r="U74" s="185"/>
+      <c r="V74" s="185"/>
+      <c r="W74" s="185"/>
+      <c r="X74" s="185"/>
+      <c r="Y74" s="185"/>
+      <c r="Z74" s="185"/>
+      <c r="AA74" s="185"/>
+      <c r="AB74" s="185"/>
+      <c r="AC74" s="185"/>
+      <c r="AD74" s="185"/>
+      <c r="AE74" s="185"/>
     </row>
     <row r="75" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A75" s="177"/>
-      <c r="B75" s="178"/>
-      <c r="C75" s="179"/>
+      <c r="A75" s="191"/>
+      <c r="B75" s="192"/>
+      <c r="C75" s="193"/>
       <c r="D75" s="217"/>
-      <c r="E75" s="203"/>
-      <c r="F75" s="203"/>
-      <c r="G75" s="203"/>
-      <c r="H75" s="203"/>
-      <c r="I75" s="203"/>
-      <c r="J75" s="203"/>
-      <c r="K75" s="203"/>
-      <c r="L75" s="203"/>
-      <c r="M75" s="203"/>
-      <c r="N75" s="203"/>
-      <c r="O75" s="203"/>
-      <c r="P75" s="203"/>
-      <c r="Q75" s="203"/>
-      <c r="R75" s="203"/>
-      <c r="S75" s="203"/>
-      <c r="T75" s="203"/>
-      <c r="U75" s="203"/>
-      <c r="V75" s="203"/>
-      <c r="W75" s="203"/>
-      <c r="X75" s="203"/>
-      <c r="Y75" s="203"/>
-      <c r="Z75" s="203"/>
-      <c r="AA75" s="203"/>
-      <c r="AB75" s="203"/>
-      <c r="AC75" s="203"/>
-      <c r="AD75" s="203"/>
-      <c r="AE75" s="203"/>
+      <c r="E75" s="185"/>
+      <c r="F75" s="185"/>
+      <c r="G75" s="185"/>
+      <c r="H75" s="185"/>
+      <c r="I75" s="185"/>
+      <c r="J75" s="185"/>
+      <c r="K75" s="185"/>
+      <c r="L75" s="185"/>
+      <c r="M75" s="185"/>
+      <c r="N75" s="185"/>
+      <c r="O75" s="185"/>
+      <c r="P75" s="185"/>
+      <c r="Q75" s="185"/>
+      <c r="R75" s="185"/>
+      <c r="S75" s="185"/>
+      <c r="T75" s="185"/>
+      <c r="U75" s="185"/>
+      <c r="V75" s="185"/>
+      <c r="W75" s="185"/>
+      <c r="X75" s="185"/>
+      <c r="Y75" s="185"/>
+      <c r="Z75" s="185"/>
+      <c r="AA75" s="185"/>
+      <c r="AB75" s="185"/>
+      <c r="AC75" s="185"/>
+      <c r="AD75" s="185"/>
+      <c r="AE75" s="185"/>
     </row>
     <row r="76" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A76" s="177"/>
-      <c r="B76" s="178"/>
-      <c r="C76" s="179"/>
+      <c r="A76" s="191"/>
+      <c r="B76" s="192"/>
+      <c r="C76" s="193"/>
       <c r="D76" s="217"/>
-      <c r="E76" s="203"/>
-      <c r="F76" s="203"/>
-      <c r="G76" s="203"/>
-      <c r="H76" s="203"/>
-      <c r="I76" s="203"/>
-      <c r="J76" s="203"/>
-      <c r="K76" s="203"/>
-      <c r="L76" s="203"/>
-      <c r="M76" s="203"/>
-      <c r="N76" s="203"/>
-      <c r="O76" s="203"/>
-      <c r="P76" s="203"/>
-      <c r="Q76" s="203"/>
-      <c r="R76" s="203"/>
-      <c r="S76" s="203"/>
-      <c r="T76" s="203"/>
-      <c r="U76" s="203"/>
-      <c r="V76" s="203"/>
-      <c r="W76" s="203"/>
-      <c r="X76" s="203"/>
-      <c r="Y76" s="203"/>
-      <c r="Z76" s="203"/>
-      <c r="AA76" s="203"/>
-      <c r="AB76" s="203"/>
-      <c r="AC76" s="203"/>
-      <c r="AD76" s="203"/>
-      <c r="AE76" s="203"/>
+      <c r="E76" s="185"/>
+      <c r="F76" s="185"/>
+      <c r="G76" s="185"/>
+      <c r="H76" s="185"/>
+      <c r="I76" s="185"/>
+      <c r="J76" s="185"/>
+      <c r="K76" s="185"/>
+      <c r="L76" s="185"/>
+      <c r="M76" s="185"/>
+      <c r="N76" s="185"/>
+      <c r="O76" s="185"/>
+      <c r="P76" s="185"/>
+      <c r="Q76" s="185"/>
+      <c r="R76" s="185"/>
+      <c r="S76" s="185"/>
+      <c r="T76" s="185"/>
+      <c r="U76" s="185"/>
+      <c r="V76" s="185"/>
+      <c r="W76" s="185"/>
+      <c r="X76" s="185"/>
+      <c r="Y76" s="185"/>
+      <c r="Z76" s="185"/>
+      <c r="AA76" s="185"/>
+      <c r="AB76" s="185"/>
+      <c r="AC76" s="185"/>
+      <c r="AD76" s="185"/>
+      <c r="AE76" s="185"/>
     </row>
     <row r="77" spans="1:31" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A77" s="180"/>
-      <c r="B77" s="181"/>
-      <c r="C77" s="182"/>
+      <c r="A77" s="194"/>
+      <c r="B77" s="195"/>
+      <c r="C77" s="196"/>
       <c r="D77" s="219"/>
       <c r="E77" s="216"/>
       <c r="F77" s="216"/>
@@ -7263,9 +7299,9 @@
       <c r="AE77" s="216"/>
     </row>
     <row r="78" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A78" s="172"/>
-      <c r="B78" s="173"/>
-      <c r="C78" s="176"/>
+      <c r="A78" s="188"/>
+      <c r="B78" s="189"/>
+      <c r="C78" s="190"/>
       <c r="D78" s="218"/>
       <c r="E78" s="214"/>
       <c r="F78" s="214"/>
@@ -7296,108 +7332,108 @@
       <c r="AE78" s="214"/>
     </row>
     <row r="79" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A79" s="177"/>
-      <c r="B79" s="178"/>
-      <c r="C79" s="179"/>
+      <c r="A79" s="191"/>
+      <c r="B79" s="192"/>
+      <c r="C79" s="193"/>
       <c r="D79" s="217"/>
-      <c r="E79" s="203"/>
-      <c r="F79" s="203"/>
-      <c r="G79" s="203"/>
-      <c r="H79" s="203"/>
-      <c r="I79" s="203"/>
-      <c r="J79" s="203"/>
-      <c r="K79" s="203"/>
-      <c r="L79" s="203"/>
-      <c r="M79" s="203"/>
-      <c r="N79" s="203"/>
-      <c r="O79" s="203"/>
-      <c r="P79" s="203"/>
-      <c r="Q79" s="203"/>
-      <c r="R79" s="203"/>
-      <c r="S79" s="203"/>
-      <c r="T79" s="203"/>
-      <c r="U79" s="203"/>
-      <c r="V79" s="203"/>
-      <c r="W79" s="203"/>
-      <c r="X79" s="203"/>
-      <c r="Y79" s="203"/>
-      <c r="Z79" s="203"/>
-      <c r="AA79" s="203"/>
-      <c r="AB79" s="203"/>
-      <c r="AC79" s="203"/>
-      <c r="AD79" s="203"/>
-      <c r="AE79" s="203"/>
+      <c r="E79" s="185"/>
+      <c r="F79" s="185"/>
+      <c r="G79" s="185"/>
+      <c r="H79" s="185"/>
+      <c r="I79" s="185"/>
+      <c r="J79" s="185"/>
+      <c r="K79" s="185"/>
+      <c r="L79" s="185"/>
+      <c r="M79" s="185"/>
+      <c r="N79" s="185"/>
+      <c r="O79" s="185"/>
+      <c r="P79" s="185"/>
+      <c r="Q79" s="185"/>
+      <c r="R79" s="185"/>
+      <c r="S79" s="185"/>
+      <c r="T79" s="185"/>
+      <c r="U79" s="185"/>
+      <c r="V79" s="185"/>
+      <c r="W79" s="185"/>
+      <c r="X79" s="185"/>
+      <c r="Y79" s="185"/>
+      <c r="Z79" s="185"/>
+      <c r="AA79" s="185"/>
+      <c r="AB79" s="185"/>
+      <c r="AC79" s="185"/>
+      <c r="AD79" s="185"/>
+      <c r="AE79" s="185"/>
     </row>
     <row r="80" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A80" s="177"/>
-      <c r="B80" s="178"/>
-      <c r="C80" s="179"/>
+      <c r="A80" s="191"/>
+      <c r="B80" s="192"/>
+      <c r="C80" s="193"/>
       <c r="D80" s="217"/>
-      <c r="E80" s="203"/>
-      <c r="F80" s="203"/>
-      <c r="G80" s="203"/>
-      <c r="H80" s="203"/>
-      <c r="I80" s="203"/>
-      <c r="J80" s="203"/>
-      <c r="K80" s="203"/>
-      <c r="L80" s="203"/>
-      <c r="M80" s="203"/>
-      <c r="N80" s="203"/>
-      <c r="O80" s="203"/>
-      <c r="P80" s="203"/>
-      <c r="Q80" s="203"/>
-      <c r="R80" s="203"/>
-      <c r="S80" s="203"/>
-      <c r="T80" s="203"/>
-      <c r="U80" s="203"/>
-      <c r="V80" s="203"/>
-      <c r="W80" s="203"/>
-      <c r="X80" s="203"/>
-      <c r="Y80" s="203"/>
-      <c r="Z80" s="203"/>
-      <c r="AA80" s="203"/>
-      <c r="AB80" s="203"/>
-      <c r="AC80" s="203"/>
-      <c r="AD80" s="203"/>
-      <c r="AE80" s="203"/>
+      <c r="E80" s="185"/>
+      <c r="F80" s="185"/>
+      <c r="G80" s="185"/>
+      <c r="H80" s="185"/>
+      <c r="I80" s="185"/>
+      <c r="J80" s="185"/>
+      <c r="K80" s="185"/>
+      <c r="L80" s="185"/>
+      <c r="M80" s="185"/>
+      <c r="N80" s="185"/>
+      <c r="O80" s="185"/>
+      <c r="P80" s="185"/>
+      <c r="Q80" s="185"/>
+      <c r="R80" s="185"/>
+      <c r="S80" s="185"/>
+      <c r="T80" s="185"/>
+      <c r="U80" s="185"/>
+      <c r="V80" s="185"/>
+      <c r="W80" s="185"/>
+      <c r="X80" s="185"/>
+      <c r="Y80" s="185"/>
+      <c r="Z80" s="185"/>
+      <c r="AA80" s="185"/>
+      <c r="AB80" s="185"/>
+      <c r="AC80" s="185"/>
+      <c r="AD80" s="185"/>
+      <c r="AE80" s="185"/>
     </row>
     <row r="81" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A81" s="177"/>
-      <c r="B81" s="178"/>
-      <c r="C81" s="179"/>
+      <c r="A81" s="191"/>
+      <c r="B81" s="192"/>
+      <c r="C81" s="193"/>
       <c r="D81" s="217"/>
-      <c r="E81" s="203"/>
-      <c r="F81" s="203"/>
-      <c r="G81" s="203"/>
-      <c r="H81" s="203"/>
-      <c r="I81" s="203"/>
-      <c r="J81" s="203"/>
-      <c r="K81" s="203"/>
-      <c r="L81" s="203"/>
-      <c r="M81" s="203"/>
-      <c r="N81" s="203"/>
-      <c r="O81" s="203"/>
-      <c r="P81" s="203"/>
-      <c r="Q81" s="203"/>
-      <c r="R81" s="203"/>
-      <c r="S81" s="203"/>
-      <c r="T81" s="203"/>
-      <c r="U81" s="203"/>
-      <c r="V81" s="203"/>
-      <c r="W81" s="203"/>
-      <c r="X81" s="203"/>
-      <c r="Y81" s="203"/>
-      <c r="Z81" s="203"/>
-      <c r="AA81" s="203"/>
-      <c r="AB81" s="203"/>
-      <c r="AC81" s="203"/>
-      <c r="AD81" s="203"/>
-      <c r="AE81" s="203"/>
+      <c r="E81" s="185"/>
+      <c r="F81" s="185"/>
+      <c r="G81" s="185"/>
+      <c r="H81" s="185"/>
+      <c r="I81" s="185"/>
+      <c r="J81" s="185"/>
+      <c r="K81" s="185"/>
+      <c r="L81" s="185"/>
+      <c r="M81" s="185"/>
+      <c r="N81" s="185"/>
+      <c r="O81" s="185"/>
+      <c r="P81" s="185"/>
+      <c r="Q81" s="185"/>
+      <c r="R81" s="185"/>
+      <c r="S81" s="185"/>
+      <c r="T81" s="185"/>
+      <c r="U81" s="185"/>
+      <c r="V81" s="185"/>
+      <c r="W81" s="185"/>
+      <c r="X81" s="185"/>
+      <c r="Y81" s="185"/>
+      <c r="Z81" s="185"/>
+      <c r="AA81" s="185"/>
+      <c r="AB81" s="185"/>
+      <c r="AC81" s="185"/>
+      <c r="AD81" s="185"/>
+      <c r="AE81" s="185"/>
     </row>
     <row r="82" spans="1:31" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A82" s="180"/>
-      <c r="B82" s="181"/>
-      <c r="C82" s="182"/>
+      <c r="A82" s="194"/>
+      <c r="B82" s="195"/>
+      <c r="C82" s="196"/>
       <c r="D82" s="219"/>
       <c r="E82" s="216"/>
       <c r="F82" s="216"/>
@@ -7428,9 +7464,9 @@
       <c r="AE82" s="216"/>
     </row>
     <row r="83" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A83" s="172"/>
-      <c r="B83" s="173"/>
-      <c r="C83" s="176"/>
+      <c r="A83" s="188"/>
+      <c r="B83" s="189"/>
+      <c r="C83" s="190"/>
       <c r="D83" s="218"/>
       <c r="E83" s="214"/>
       <c r="F83" s="214"/>
@@ -7461,108 +7497,108 @@
       <c r="AE83" s="214"/>
     </row>
     <row r="84" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A84" s="177"/>
-      <c r="B84" s="178"/>
-      <c r="C84" s="179"/>
+      <c r="A84" s="191"/>
+      <c r="B84" s="192"/>
+      <c r="C84" s="193"/>
       <c r="D84" s="217"/>
-      <c r="E84" s="203"/>
-      <c r="F84" s="203"/>
-      <c r="G84" s="203"/>
-      <c r="H84" s="203"/>
-      <c r="I84" s="203"/>
-      <c r="J84" s="203"/>
-      <c r="K84" s="203"/>
-      <c r="L84" s="203"/>
-      <c r="M84" s="203"/>
-      <c r="N84" s="203"/>
-      <c r="O84" s="203"/>
-      <c r="P84" s="203"/>
-      <c r="Q84" s="203"/>
-      <c r="R84" s="203"/>
-      <c r="S84" s="203"/>
-      <c r="T84" s="203"/>
-      <c r="U84" s="203"/>
-      <c r="V84" s="203"/>
-      <c r="W84" s="203"/>
-      <c r="X84" s="203"/>
-      <c r="Y84" s="203"/>
-      <c r="Z84" s="203"/>
-      <c r="AA84" s="203"/>
-      <c r="AB84" s="203"/>
-      <c r="AC84" s="203"/>
-      <c r="AD84" s="203"/>
-      <c r="AE84" s="203"/>
+      <c r="E84" s="185"/>
+      <c r="F84" s="185"/>
+      <c r="G84" s="185"/>
+      <c r="H84" s="185"/>
+      <c r="I84" s="185"/>
+      <c r="J84" s="185"/>
+      <c r="K84" s="185"/>
+      <c r="L84" s="185"/>
+      <c r="M84" s="185"/>
+      <c r="N84" s="185"/>
+      <c r="O84" s="185"/>
+      <c r="P84" s="185"/>
+      <c r="Q84" s="185"/>
+      <c r="R84" s="185"/>
+      <c r="S84" s="185"/>
+      <c r="T84" s="185"/>
+      <c r="U84" s="185"/>
+      <c r="V84" s="185"/>
+      <c r="W84" s="185"/>
+      <c r="X84" s="185"/>
+      <c r="Y84" s="185"/>
+      <c r="Z84" s="185"/>
+      <c r="AA84" s="185"/>
+      <c r="AB84" s="185"/>
+      <c r="AC84" s="185"/>
+      <c r="AD84" s="185"/>
+      <c r="AE84" s="185"/>
     </row>
     <row r="85" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A85" s="177"/>
-      <c r="B85" s="178"/>
-      <c r="C85" s="179"/>
+      <c r="A85" s="191"/>
+      <c r="B85" s="192"/>
+      <c r="C85" s="193"/>
       <c r="D85" s="217"/>
-      <c r="E85" s="203"/>
-      <c r="F85" s="203"/>
-      <c r="G85" s="203"/>
-      <c r="H85" s="203"/>
-      <c r="I85" s="203"/>
-      <c r="J85" s="203"/>
-      <c r="K85" s="203"/>
-      <c r="L85" s="203"/>
-      <c r="M85" s="203"/>
-      <c r="N85" s="203"/>
-      <c r="O85" s="203"/>
-      <c r="P85" s="203"/>
-      <c r="Q85" s="203"/>
-      <c r="R85" s="203"/>
-      <c r="S85" s="203"/>
-      <c r="T85" s="203"/>
-      <c r="U85" s="203"/>
-      <c r="V85" s="203"/>
-      <c r="W85" s="203"/>
-      <c r="X85" s="203"/>
-      <c r="Y85" s="203"/>
-      <c r="Z85" s="203"/>
-      <c r="AA85" s="203"/>
-      <c r="AB85" s="203"/>
-      <c r="AC85" s="203"/>
-      <c r="AD85" s="203"/>
-      <c r="AE85" s="203"/>
+      <c r="E85" s="185"/>
+      <c r="F85" s="185"/>
+      <c r="G85" s="185"/>
+      <c r="H85" s="185"/>
+      <c r="I85" s="185"/>
+      <c r="J85" s="185"/>
+      <c r="K85" s="185"/>
+      <c r="L85" s="185"/>
+      <c r="M85" s="185"/>
+      <c r="N85" s="185"/>
+      <c r="O85" s="185"/>
+      <c r="P85" s="185"/>
+      <c r="Q85" s="185"/>
+      <c r="R85" s="185"/>
+      <c r="S85" s="185"/>
+      <c r="T85" s="185"/>
+      <c r="U85" s="185"/>
+      <c r="V85" s="185"/>
+      <c r="W85" s="185"/>
+      <c r="X85" s="185"/>
+      <c r="Y85" s="185"/>
+      <c r="Z85" s="185"/>
+      <c r="AA85" s="185"/>
+      <c r="AB85" s="185"/>
+      <c r="AC85" s="185"/>
+      <c r="AD85" s="185"/>
+      <c r="AE85" s="185"/>
     </row>
     <row r="86" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A86" s="177"/>
-      <c r="B86" s="178"/>
-      <c r="C86" s="179"/>
+      <c r="A86" s="191"/>
+      <c r="B86" s="192"/>
+      <c r="C86" s="193"/>
       <c r="D86" s="217"/>
-      <c r="E86" s="203"/>
-      <c r="F86" s="203"/>
-      <c r="G86" s="203"/>
-      <c r="H86" s="203"/>
-      <c r="I86" s="203"/>
-      <c r="J86" s="203"/>
-      <c r="K86" s="203"/>
-      <c r="L86" s="203"/>
-      <c r="M86" s="203"/>
-      <c r="N86" s="203"/>
-      <c r="O86" s="203"/>
-      <c r="P86" s="203"/>
-      <c r="Q86" s="203"/>
-      <c r="R86" s="203"/>
-      <c r="S86" s="203"/>
-      <c r="T86" s="203"/>
-      <c r="U86" s="203"/>
-      <c r="V86" s="203"/>
-      <c r="W86" s="203"/>
-      <c r="X86" s="203"/>
-      <c r="Y86" s="203"/>
-      <c r="Z86" s="203"/>
-      <c r="AA86" s="203"/>
-      <c r="AB86" s="203"/>
-      <c r="AC86" s="203"/>
-      <c r="AD86" s="203"/>
-      <c r="AE86" s="203"/>
+      <c r="E86" s="185"/>
+      <c r="F86" s="185"/>
+      <c r="G86" s="185"/>
+      <c r="H86" s="185"/>
+      <c r="I86" s="185"/>
+      <c r="J86" s="185"/>
+      <c r="K86" s="185"/>
+      <c r="L86" s="185"/>
+      <c r="M86" s="185"/>
+      <c r="N86" s="185"/>
+      <c r="O86" s="185"/>
+      <c r="P86" s="185"/>
+      <c r="Q86" s="185"/>
+      <c r="R86" s="185"/>
+      <c r="S86" s="185"/>
+      <c r="T86" s="185"/>
+      <c r="U86" s="185"/>
+      <c r="V86" s="185"/>
+      <c r="W86" s="185"/>
+      <c r="X86" s="185"/>
+      <c r="Y86" s="185"/>
+      <c r="Z86" s="185"/>
+      <c r="AA86" s="185"/>
+      <c r="AB86" s="185"/>
+      <c r="AC86" s="185"/>
+      <c r="AD86" s="185"/>
+      <c r="AE86" s="185"/>
     </row>
     <row r="87" spans="1:31" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A87" s="180"/>
-      <c r="B87" s="181"/>
-      <c r="C87" s="182"/>
+      <c r="A87" s="194"/>
+      <c r="B87" s="195"/>
+      <c r="C87" s="196"/>
       <c r="D87" s="219"/>
       <c r="E87" s="216"/>
       <c r="F87" s="216"/>
@@ -7593,9 +7629,9 @@
       <c r="AE87" s="216"/>
     </row>
     <row r="88" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A88" s="172"/>
-      <c r="B88" s="173"/>
-      <c r="C88" s="176"/>
+      <c r="A88" s="188"/>
+      <c r="B88" s="189"/>
+      <c r="C88" s="190"/>
       <c r="D88" s="218"/>
       <c r="E88" s="214"/>
       <c r="F88" s="214"/>
@@ -7626,108 +7662,108 @@
       <c r="AE88" s="214"/>
     </row>
     <row r="89" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A89" s="177"/>
-      <c r="B89" s="178"/>
-      <c r="C89" s="179"/>
+      <c r="A89" s="191"/>
+      <c r="B89" s="192"/>
+      <c r="C89" s="193"/>
       <c r="D89" s="217"/>
-      <c r="E89" s="203"/>
-      <c r="F89" s="203"/>
-      <c r="G89" s="203"/>
-      <c r="H89" s="203"/>
-      <c r="I89" s="203"/>
-      <c r="J89" s="203"/>
-      <c r="K89" s="203"/>
-      <c r="L89" s="203"/>
-      <c r="M89" s="203"/>
-      <c r="N89" s="203"/>
-      <c r="O89" s="203"/>
-      <c r="P89" s="203"/>
-      <c r="Q89" s="203"/>
-      <c r="R89" s="203"/>
-      <c r="S89" s="203"/>
-      <c r="T89" s="203"/>
-      <c r="U89" s="203"/>
-      <c r="V89" s="203"/>
-      <c r="W89" s="203"/>
-      <c r="X89" s="203"/>
-      <c r="Y89" s="203"/>
-      <c r="Z89" s="203"/>
-      <c r="AA89" s="203"/>
-      <c r="AB89" s="203"/>
-      <c r="AC89" s="203"/>
-      <c r="AD89" s="203"/>
-      <c r="AE89" s="203"/>
+      <c r="E89" s="185"/>
+      <c r="F89" s="185"/>
+      <c r="G89" s="185"/>
+      <c r="H89" s="185"/>
+      <c r="I89" s="185"/>
+      <c r="J89" s="185"/>
+      <c r="K89" s="185"/>
+      <c r="L89" s="185"/>
+      <c r="M89" s="185"/>
+      <c r="N89" s="185"/>
+      <c r="O89" s="185"/>
+      <c r="P89" s="185"/>
+      <c r="Q89" s="185"/>
+      <c r="R89" s="185"/>
+      <c r="S89" s="185"/>
+      <c r="T89" s="185"/>
+      <c r="U89" s="185"/>
+      <c r="V89" s="185"/>
+      <c r="W89" s="185"/>
+      <c r="X89" s="185"/>
+      <c r="Y89" s="185"/>
+      <c r="Z89" s="185"/>
+      <c r="AA89" s="185"/>
+      <c r="AB89" s="185"/>
+      <c r="AC89" s="185"/>
+      <c r="AD89" s="185"/>
+      <c r="AE89" s="185"/>
     </row>
     <row r="90" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A90" s="177"/>
-      <c r="B90" s="178"/>
-      <c r="C90" s="179"/>
+      <c r="A90" s="191"/>
+      <c r="B90" s="192"/>
+      <c r="C90" s="193"/>
       <c r="D90" s="217"/>
-      <c r="E90" s="203"/>
-      <c r="F90" s="203"/>
-      <c r="G90" s="203"/>
-      <c r="H90" s="203"/>
-      <c r="I90" s="203"/>
-      <c r="J90" s="203"/>
-      <c r="K90" s="203"/>
-      <c r="L90" s="203"/>
-      <c r="M90" s="203"/>
-      <c r="N90" s="203"/>
-      <c r="O90" s="203"/>
-      <c r="P90" s="203"/>
-      <c r="Q90" s="203"/>
-      <c r="R90" s="203"/>
-      <c r="S90" s="203"/>
-      <c r="T90" s="203"/>
-      <c r="U90" s="203"/>
-      <c r="V90" s="203"/>
-      <c r="W90" s="203"/>
-      <c r="X90" s="203"/>
-      <c r="Y90" s="203"/>
-      <c r="Z90" s="203"/>
-      <c r="AA90" s="203"/>
-      <c r="AB90" s="203"/>
-      <c r="AC90" s="203"/>
-      <c r="AD90" s="203"/>
-      <c r="AE90" s="203"/>
+      <c r="E90" s="185"/>
+      <c r="F90" s="185"/>
+      <c r="G90" s="185"/>
+      <c r="H90" s="185"/>
+      <c r="I90" s="185"/>
+      <c r="J90" s="185"/>
+      <c r="K90" s="185"/>
+      <c r="L90" s="185"/>
+      <c r="M90" s="185"/>
+      <c r="N90" s="185"/>
+      <c r="O90" s="185"/>
+      <c r="P90" s="185"/>
+      <c r="Q90" s="185"/>
+      <c r="R90" s="185"/>
+      <c r="S90" s="185"/>
+      <c r="T90" s="185"/>
+      <c r="U90" s="185"/>
+      <c r="V90" s="185"/>
+      <c r="W90" s="185"/>
+      <c r="X90" s="185"/>
+      <c r="Y90" s="185"/>
+      <c r="Z90" s="185"/>
+      <c r="AA90" s="185"/>
+      <c r="AB90" s="185"/>
+      <c r="AC90" s="185"/>
+      <c r="AD90" s="185"/>
+      <c r="AE90" s="185"/>
     </row>
     <row r="91" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A91" s="177"/>
-      <c r="B91" s="178"/>
-      <c r="C91" s="179"/>
+      <c r="A91" s="191"/>
+      <c r="B91" s="192"/>
+      <c r="C91" s="193"/>
       <c r="D91" s="217"/>
-      <c r="E91" s="203"/>
-      <c r="F91" s="203"/>
-      <c r="G91" s="203"/>
-      <c r="H91" s="203"/>
-      <c r="I91" s="203"/>
-      <c r="J91" s="203"/>
-      <c r="K91" s="203"/>
-      <c r="L91" s="203"/>
-      <c r="M91" s="203"/>
-      <c r="N91" s="203"/>
-      <c r="O91" s="203"/>
-      <c r="P91" s="203"/>
-      <c r="Q91" s="203"/>
-      <c r="R91" s="203"/>
-      <c r="S91" s="203"/>
-      <c r="T91" s="203"/>
-      <c r="U91" s="203"/>
-      <c r="V91" s="203"/>
-      <c r="W91" s="203"/>
-      <c r="X91" s="203"/>
-      <c r="Y91" s="203"/>
-      <c r="Z91" s="203"/>
-      <c r="AA91" s="203"/>
-      <c r="AB91" s="203"/>
-      <c r="AC91" s="203"/>
-      <c r="AD91" s="203"/>
-      <c r="AE91" s="203"/>
+      <c r="E91" s="185"/>
+      <c r="F91" s="185"/>
+      <c r="G91" s="185"/>
+      <c r="H91" s="185"/>
+      <c r="I91" s="185"/>
+      <c r="J91" s="185"/>
+      <c r="K91" s="185"/>
+      <c r="L91" s="185"/>
+      <c r="M91" s="185"/>
+      <c r="N91" s="185"/>
+      <c r="O91" s="185"/>
+      <c r="P91" s="185"/>
+      <c r="Q91" s="185"/>
+      <c r="R91" s="185"/>
+      <c r="S91" s="185"/>
+      <c r="T91" s="185"/>
+      <c r="U91" s="185"/>
+      <c r="V91" s="185"/>
+      <c r="W91" s="185"/>
+      <c r="X91" s="185"/>
+      <c r="Y91" s="185"/>
+      <c r="Z91" s="185"/>
+      <c r="AA91" s="185"/>
+      <c r="AB91" s="185"/>
+      <c r="AC91" s="185"/>
+      <c r="AD91" s="185"/>
+      <c r="AE91" s="185"/>
     </row>
     <row r="92" spans="1:31" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A92" s="180"/>
-      <c r="B92" s="181"/>
-      <c r="C92" s="182"/>
+      <c r="A92" s="194"/>
+      <c r="B92" s="195"/>
+      <c r="C92" s="196"/>
       <c r="D92" s="219"/>
       <c r="E92" s="216"/>
       <c r="F92" s="216"/>
@@ -7758,9 +7794,9 @@
       <c r="AE92" s="216"/>
     </row>
     <row r="93" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A93" s="172"/>
-      <c r="B93" s="173"/>
-      <c r="C93" s="176"/>
+      <c r="A93" s="188"/>
+      <c r="B93" s="189"/>
+      <c r="C93" s="190"/>
       <c r="D93" s="218"/>
       <c r="E93" s="214"/>
       <c r="F93" s="214"/>
@@ -7791,108 +7827,108 @@
       <c r="AE93" s="214"/>
     </row>
     <row r="94" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A94" s="177"/>
-      <c r="B94" s="178"/>
-      <c r="C94" s="179"/>
+      <c r="A94" s="191"/>
+      <c r="B94" s="192"/>
+      <c r="C94" s="193"/>
       <c r="D94" s="217"/>
-      <c r="E94" s="203"/>
-      <c r="F94" s="203"/>
-      <c r="G94" s="203"/>
-      <c r="H94" s="203"/>
-      <c r="I94" s="203"/>
-      <c r="J94" s="203"/>
-      <c r="K94" s="203"/>
-      <c r="L94" s="203"/>
-      <c r="M94" s="203"/>
-      <c r="N94" s="203"/>
-      <c r="O94" s="203"/>
-      <c r="P94" s="203"/>
-      <c r="Q94" s="203"/>
-      <c r="R94" s="203"/>
-      <c r="S94" s="203"/>
-      <c r="T94" s="203"/>
-      <c r="U94" s="203"/>
-      <c r="V94" s="203"/>
-      <c r="W94" s="203"/>
-      <c r="X94" s="203"/>
-      <c r="Y94" s="203"/>
-      <c r="Z94" s="203"/>
-      <c r="AA94" s="203"/>
-      <c r="AB94" s="203"/>
-      <c r="AC94" s="203"/>
-      <c r="AD94" s="203"/>
-      <c r="AE94" s="203"/>
+      <c r="E94" s="185"/>
+      <c r="F94" s="185"/>
+      <c r="G94" s="185"/>
+      <c r="H94" s="185"/>
+      <c r="I94" s="185"/>
+      <c r="J94" s="185"/>
+      <c r="K94" s="185"/>
+      <c r="L94" s="185"/>
+      <c r="M94" s="185"/>
+      <c r="N94" s="185"/>
+      <c r="O94" s="185"/>
+      <c r="P94" s="185"/>
+      <c r="Q94" s="185"/>
+      <c r="R94" s="185"/>
+      <c r="S94" s="185"/>
+      <c r="T94" s="185"/>
+      <c r="U94" s="185"/>
+      <c r="V94" s="185"/>
+      <c r="W94" s="185"/>
+      <c r="X94" s="185"/>
+      <c r="Y94" s="185"/>
+      <c r="Z94" s="185"/>
+      <c r="AA94" s="185"/>
+      <c r="AB94" s="185"/>
+      <c r="AC94" s="185"/>
+      <c r="AD94" s="185"/>
+      <c r="AE94" s="185"/>
     </row>
     <row r="95" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A95" s="177"/>
-      <c r="B95" s="178"/>
-      <c r="C95" s="179"/>
+      <c r="A95" s="191"/>
+      <c r="B95" s="192"/>
+      <c r="C95" s="193"/>
       <c r="D95" s="217"/>
-      <c r="E95" s="203"/>
-      <c r="F95" s="203"/>
-      <c r="G95" s="203"/>
-      <c r="H95" s="203"/>
-      <c r="I95" s="203"/>
-      <c r="J95" s="203"/>
-      <c r="K95" s="203"/>
-      <c r="L95" s="203"/>
-      <c r="M95" s="203"/>
-      <c r="N95" s="203"/>
-      <c r="O95" s="203"/>
-      <c r="P95" s="203"/>
-      <c r="Q95" s="203"/>
-      <c r="R95" s="203"/>
-      <c r="S95" s="203"/>
-      <c r="T95" s="203"/>
-      <c r="U95" s="203"/>
-      <c r="V95" s="203"/>
-      <c r="W95" s="203"/>
-      <c r="X95" s="203"/>
-      <c r="Y95" s="203"/>
-      <c r="Z95" s="203"/>
-      <c r="AA95" s="203"/>
-      <c r="AB95" s="203"/>
-      <c r="AC95" s="203"/>
-      <c r="AD95" s="203"/>
-      <c r="AE95" s="203"/>
+      <c r="E95" s="185"/>
+      <c r="F95" s="185"/>
+      <c r="G95" s="185"/>
+      <c r="H95" s="185"/>
+      <c r="I95" s="185"/>
+      <c r="J95" s="185"/>
+      <c r="K95" s="185"/>
+      <c r="L95" s="185"/>
+      <c r="M95" s="185"/>
+      <c r="N95" s="185"/>
+      <c r="O95" s="185"/>
+      <c r="P95" s="185"/>
+      <c r="Q95" s="185"/>
+      <c r="R95" s="185"/>
+      <c r="S95" s="185"/>
+      <c r="T95" s="185"/>
+      <c r="U95" s="185"/>
+      <c r="V95" s="185"/>
+      <c r="W95" s="185"/>
+      <c r="X95" s="185"/>
+      <c r="Y95" s="185"/>
+      <c r="Z95" s="185"/>
+      <c r="AA95" s="185"/>
+      <c r="AB95" s="185"/>
+      <c r="AC95" s="185"/>
+      <c r="AD95" s="185"/>
+      <c r="AE95" s="185"/>
     </row>
     <row r="96" spans="1:31" ht="11.25" customHeight="1">
-      <c r="A96" s="177"/>
-      <c r="B96" s="178"/>
-      <c r="C96" s="179"/>
+      <c r="A96" s="191"/>
+      <c r="B96" s="192"/>
+      <c r="C96" s="193"/>
       <c r="D96" s="217"/>
-      <c r="E96" s="203"/>
-      <c r="F96" s="203"/>
-      <c r="G96" s="203"/>
-      <c r="H96" s="203"/>
-      <c r="I96" s="203"/>
-      <c r="J96" s="203"/>
-      <c r="K96" s="203"/>
-      <c r="L96" s="203"/>
-      <c r="M96" s="203"/>
-      <c r="N96" s="203"/>
-      <c r="O96" s="203"/>
-      <c r="P96" s="203"/>
-      <c r="Q96" s="203"/>
-      <c r="R96" s="203"/>
-      <c r="S96" s="203"/>
-      <c r="T96" s="203"/>
-      <c r="U96" s="203"/>
-      <c r="V96" s="203"/>
-      <c r="W96" s="203"/>
-      <c r="X96" s="203"/>
-      <c r="Y96" s="203"/>
-      <c r="Z96" s="203"/>
-      <c r="AA96" s="203"/>
-      <c r="AB96" s="203"/>
-      <c r="AC96" s="203"/>
-      <c r="AD96" s="203"/>
-      <c r="AE96" s="203"/>
+      <c r="E96" s="185"/>
+      <c r="F96" s="185"/>
+      <c r="G96" s="185"/>
+      <c r="H96" s="185"/>
+      <c r="I96" s="185"/>
+      <c r="J96" s="185"/>
+      <c r="K96" s="185"/>
+      <c r="L96" s="185"/>
+      <c r="M96" s="185"/>
+      <c r="N96" s="185"/>
+      <c r="O96" s="185"/>
+      <c r="P96" s="185"/>
+      <c r="Q96" s="185"/>
+      <c r="R96" s="185"/>
+      <c r="S96" s="185"/>
+      <c r="T96" s="185"/>
+      <c r="U96" s="185"/>
+      <c r="V96" s="185"/>
+      <c r="W96" s="185"/>
+      <c r="X96" s="185"/>
+      <c r="Y96" s="185"/>
+      <c r="Z96" s="185"/>
+      <c r="AA96" s="185"/>
+      <c r="AB96" s="185"/>
+      <c r="AC96" s="185"/>
+      <c r="AD96" s="185"/>
+      <c r="AE96" s="185"/>
     </row>
     <row r="97" spans="1:31" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A97" s="180"/>
-      <c r="B97" s="181"/>
-      <c r="C97" s="182"/>
+      <c r="A97" s="194"/>
+      <c r="B97" s="195"/>
+      <c r="C97" s="196"/>
       <c r="D97" s="219"/>
       <c r="E97" s="216"/>
       <c r="F97" s="216"/>
@@ -8006,6 +8042,7 @@
     <mergeCell ref="T30:U30"/>
     <mergeCell ref="X30:Y30"/>
     <mergeCell ref="V30:W30"/>
+    <mergeCell ref="P31:U31"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="R52:S52"/>
@@ -8619,20 +8656,6 @@
     <mergeCell ref="T87:U87"/>
     <mergeCell ref="V87:W87"/>
     <mergeCell ref="X87:Y87"/>
-    <mergeCell ref="AB53:AC53"/>
-    <mergeCell ref="R51:S51"/>
-    <mergeCell ref="AD51:AE51"/>
-    <mergeCell ref="AD49:AE49"/>
-    <mergeCell ref="AD48:AE48"/>
-    <mergeCell ref="AB49:AC49"/>
-    <mergeCell ref="Z49:AA49"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="AB48:AC48"/>
-    <mergeCell ref="V49:W49"/>
-    <mergeCell ref="X49:Y49"/>
-    <mergeCell ref="AB51:AC51"/>
     <mergeCell ref="AB52:AC52"/>
     <mergeCell ref="X52:Y52"/>
     <mergeCell ref="V52:W52"/>
@@ -8643,7 +8666,15 @@
     <mergeCell ref="L52:M52"/>
     <mergeCell ref="N52:O52"/>
     <mergeCell ref="T52:U52"/>
-    <mergeCell ref="P31:U31"/>
+    <mergeCell ref="AB49:AC49"/>
+    <mergeCell ref="Z49:AA49"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="AB48:AC48"/>
+    <mergeCell ref="V49:W49"/>
+    <mergeCell ref="X49:Y49"/>
+    <mergeCell ref="AB51:AC51"/>
     <mergeCell ref="X31:Y31"/>
     <mergeCell ref="AB31:AC31"/>
     <mergeCell ref="Z39:AA39"/>
@@ -8694,6 +8725,11 @@
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="J49:K49"/>
     <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="AB53:AC53"/>
+    <mergeCell ref="R51:S51"/>
+    <mergeCell ref="AD51:AE51"/>
+    <mergeCell ref="AD49:AE49"/>
+    <mergeCell ref="AD48:AE48"/>
     <mergeCell ref="V29:AE29"/>
     <mergeCell ref="P28:AE28"/>
     <mergeCell ref="AD31:AE31"/>
@@ -8853,34 +8889,34 @@
         <v>27</v>
       </c>
       <c r="B4" s="25"/>
-      <c r="C4" s="260"/>
+      <c r="C4" s="261"/>
       <c r="D4" s="257"/>
-      <c r="E4" s="261"/>
+      <c r="E4" s="259"/>
       <c r="F4" s="257"/>
-      <c r="G4" s="261"/>
+      <c r="G4" s="259"/>
       <c r="H4" s="257"/>
-      <c r="I4" s="261"/>
+      <c r="I4" s="259"/>
       <c r="J4" s="257"/>
-      <c r="K4" s="261"/>
+      <c r="K4" s="259"/>
       <c r="L4" s="257"/>
-      <c r="M4" s="261"/>
+      <c r="M4" s="259"/>
       <c r="N4" s="257"/>
-      <c r="O4" s="261"/>
+      <c r="O4" s="259"/>
       <c r="P4" s="257"/>
-      <c r="Q4" s="261"/>
+      <c r="Q4" s="259"/>
       <c r="R4" s="257"/>
-      <c r="S4" s="261"/>
+      <c r="S4" s="259"/>
       <c r="T4" s="257"/>
-      <c r="U4" s="261"/>
+      <c r="U4" s="259"/>
       <c r="V4" s="257"/>
       <c r="W4" s="21"/>
       <c r="X4" s="16"/>
-      <c r="Y4" s="261"/>
+      <c r="Y4" s="259"/>
       <c r="Z4" s="257"/>
-      <c r="AA4" s="261"/>
+      <c r="AA4" s="259"/>
       <c r="AB4" s="257"/>
-      <c r="AC4" s="261"/>
-      <c r="AD4" s="268"/>
+      <c r="AC4" s="259"/>
+      <c r="AD4" s="260"/>
     </row>
     <row r="5" spans="1:30" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A5" s="18" t="s">
@@ -9158,33 +9194,33 @@
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="267"/>
-      <c r="D13" s="259"/>
-      <c r="E13" s="259"/>
-      <c r="F13" s="259"/>
-      <c r="G13" s="259"/>
-      <c r="H13" s="259"/>
-      <c r="I13" s="259"/>
-      <c r="J13" s="259"/>
-      <c r="K13" s="259"/>
-      <c r="L13" s="259"/>
-      <c r="M13" s="259"/>
-      <c r="N13" s="259"/>
-      <c r="O13" s="259"/>
-      <c r="P13" s="259"/>
-      <c r="Q13" s="259"/>
-      <c r="R13" s="259"/>
-      <c r="S13" s="259"/>
-      <c r="T13" s="259"/>
-      <c r="U13" s="259"/>
-      <c r="V13" s="259"/>
+      <c r="D13" s="264"/>
+      <c r="E13" s="264"/>
+      <c r="F13" s="264"/>
+      <c r="G13" s="264"/>
+      <c r="H13" s="264"/>
+      <c r="I13" s="264"/>
+      <c r="J13" s="264"/>
+      <c r="K13" s="264"/>
+      <c r="L13" s="264"/>
+      <c r="M13" s="264"/>
+      <c r="N13" s="264"/>
+      <c r="O13" s="264"/>
+      <c r="P13" s="264"/>
+      <c r="Q13" s="264"/>
+      <c r="R13" s="264"/>
+      <c r="S13" s="264"/>
+      <c r="T13" s="264"/>
+      <c r="U13" s="264"/>
+      <c r="V13" s="264"/>
       <c r="W13" s="32"/>
       <c r="X13" s="19"/>
-      <c r="Y13" s="259"/>
-      <c r="Z13" s="259"/>
-      <c r="AA13" s="259"/>
-      <c r="AB13" s="259"/>
-      <c r="AC13" s="259"/>
-      <c r="AD13" s="269"/>
+      <c r="Y13" s="264"/>
+      <c r="Z13" s="264"/>
+      <c r="AA13" s="264"/>
+      <c r="AB13" s="264"/>
+      <c r="AC13" s="264"/>
+      <c r="AD13" s="268"/>
     </row>
     <row r="14" spans="1:30" s="1" customFormat="1" ht="20" customHeight="1" thickBot="1">
       <c r="A14" s="59" t="s">
@@ -9192,33 +9228,33 @@
       </c>
       <c r="B14" s="60"/>
       <c r="C14" s="266"/>
-      <c r="D14" s="264"/>
-      <c r="E14" s="264"/>
-      <c r="F14" s="264"/>
-      <c r="G14" s="264"/>
-      <c r="H14" s="264"/>
-      <c r="I14" s="264"/>
-      <c r="J14" s="264"/>
-      <c r="K14" s="264"/>
-      <c r="L14" s="264"/>
-      <c r="M14" s="264"/>
-      <c r="N14" s="264"/>
-      <c r="O14" s="264"/>
-      <c r="P14" s="264"/>
-      <c r="Q14" s="264"/>
-      <c r="R14" s="264"/>
-      <c r="S14" s="264"/>
-      <c r="T14" s="264"/>
-      <c r="U14" s="264"/>
-      <c r="V14" s="264"/>
+      <c r="D14" s="265"/>
+      <c r="E14" s="265"/>
+      <c r="F14" s="265"/>
+      <c r="G14" s="265"/>
+      <c r="H14" s="265"/>
+      <c r="I14" s="265"/>
+      <c r="J14" s="265"/>
+      <c r="K14" s="265"/>
+      <c r="L14" s="265"/>
+      <c r="M14" s="265"/>
+      <c r="N14" s="265"/>
+      <c r="O14" s="265"/>
+      <c r="P14" s="265"/>
+      <c r="Q14" s="265"/>
+      <c r="R14" s="265"/>
+      <c r="S14" s="265"/>
+      <c r="T14" s="265"/>
+      <c r="U14" s="265"/>
+      <c r="V14" s="265"/>
       <c r="W14" s="62"/>
       <c r="X14" s="61"/>
-      <c r="Y14" s="264"/>
-      <c r="Z14" s="264"/>
-      <c r="AA14" s="264"/>
-      <c r="AB14" s="264"/>
-      <c r="AC14" s="264"/>
-      <c r="AD14" s="265"/>
+      <c r="Y14" s="265"/>
+      <c r="Z14" s="265"/>
+      <c r="AA14" s="265"/>
+      <c r="AB14" s="265"/>
+      <c r="AC14" s="265"/>
+      <c r="AD14" s="269"/>
     </row>
     <row r="15" spans="1:30" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="B15" s="15"/>
@@ -9321,7 +9357,7 @@
       <c r="D18" s="248"/>
       <c r="E18" s="248"/>
       <c r="F18" s="248"/>
-      <c r="G18" s="261"/>
+      <c r="G18" s="259"/>
       <c r="H18" s="257"/>
       <c r="I18" s="248"/>
       <c r="J18" s="248"/>
@@ -10629,13 +10665,6 @@
     <mergeCell ref="Q25:R25"/>
     <mergeCell ref="S25:T25"/>
     <mergeCell ref="U25:V25"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="U24:V24"/>
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="Y25:Z25"/>
     <mergeCell ref="Y23:Z23"/>
@@ -10648,7 +10677,6 @@
     <mergeCell ref="O24:P24"/>
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="S24:T24"/>
-    <mergeCell ref="AC18:AD18"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="K24:L24"/>
@@ -10657,6 +10685,13 @@
     <mergeCell ref="AC23:AD23"/>
     <mergeCell ref="AA24:AB24"/>
     <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="U24:V24"/>
     <mergeCell ref="AC13:AD13"/>
     <mergeCell ref="S13:T13"/>
     <mergeCell ref="U13:V13"/>
@@ -10666,6 +10701,8 @@
     <mergeCell ref="S23:T23"/>
     <mergeCell ref="U23:V23"/>
     <mergeCell ref="W23:X23"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="AC18:AD18"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -10700,7 +10737,8 @@
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="AA13:AB13"/>
     <mergeCell ref="AC12:AD12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
@@ -10714,17 +10752,6 @@
     <mergeCell ref="U12:V12"/>
     <mergeCell ref="Y12:Z12"/>
     <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="S3:T3"/>
@@ -10737,13 +10764,6 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="U10:V10"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
@@ -10753,6 +10773,9 @@
     <mergeCell ref="Q11:R11"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="AC7:AD7"/>
     <mergeCell ref="AC9:AD9"/>
     <mergeCell ref="Y10:Z10"/>
@@ -10764,6 +10787,8 @@
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="Y9:Z9"/>
     <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
@@ -10782,6 +10807,12 @@
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="S7:T7"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
@@ -10830,6 +10861,11 @@
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="O9:P9"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="Q9:R9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.23" right="0.24" top="0.18" bottom="0.17" header="0.17" footer="0.11811023622047245"/>

</xml_diff>